<commit_message>
Definition of load curves for each cabinet
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/data/Load_curves.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/data/Load_curves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micael\git\rhtlab_MIB\Mini-projet-trey_Buchser_Joye\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E85CE9-30E7-4AB7-979A-5AAD06F5CBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A87A3A-CE61-4665-BAFE-CB35BE653232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="one_housing" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="church" sheetId="5" r:id="rId4"/>
     <sheet name="industrial" sheetId="6" r:id="rId5"/>
     <sheet name="data" sheetId="2" r:id="rId6"/>
+    <sheet name="tests" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>Haushalt</t>
   </si>
@@ -99,18 +100,54 @@
   <si>
     <t>Wochenendbetrieb</t>
   </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>Courbe N5</t>
+  </si>
+  <si>
+    <t>Courbe N1 winter</t>
+  </si>
+  <si>
+    <t>Courbe N1 winter avec valeur normalisée</t>
+  </si>
+  <si>
+    <t>conso anuelle N1</t>
+  </si>
+  <si>
+    <t>Courbe 55 summer</t>
+  </si>
+  <si>
+    <t>normalisation N1</t>
+  </si>
+  <si>
+    <t>Normalisation 55</t>
+  </si>
+  <si>
+    <t>Courbe 55 summer avec valeur normalisée</t>
+  </si>
+  <si>
+    <t>conso annuelle 55</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,51 +173,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="22">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -189,32 +196,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -223,41 +205,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -266,7 +214,16 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -275,49 +232,25 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -336,13 +269,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1423AFD3-B1FF-4ECC-97A3-6C69EC5E382E}" name="Tableau1" displayName="Tableau1" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{1423AFD3-B1FF-4ECC-97A3-6C69EC5E382E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F4A83B21-5B90-4E3A-A4C4-21CB26A32609}" name="time" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{F4A83B21-5B90-4E3A-A4C4-21CB26A32609}" name="time" dataDxfId="21">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9FC972AF-5398-4422-A201-4B4234DC1C8F}" name="winter" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{9FC972AF-5398-4422-A201-4B4234DC1C8F}" name="winter" dataDxfId="20">
       <calculatedColumnFormula>AVERAGE(data!B4:D4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{34FBB4B4-434F-4EEA-9B5E-62332F1AC62D}" name="summer" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{34FBB4B4-434F-4EEA-9B5E-62332F1AC62D}" name="summer" dataDxfId="19">
       <calculatedColumnFormula>AVERAGE(data!E4:G4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -354,13 +287,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3C8F13B-6B46-4563-B8EA-AC8CEE0E4FF4}" name="Tableau13" displayName="Tableau13" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{C3C8F13B-6B46-4563-B8EA-AC8CEE0E4FF4}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{792905A5-8492-44CE-BA07-2BE3F5926705}" name="time" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{792905A5-8492-44CE-BA07-2BE3F5926705}" name="time" dataDxfId="18">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{057D2796-C49B-4646-B908-BAB657B80C5A}" name="winter" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{057D2796-C49B-4646-B908-BAB657B80C5A}" name="winter" dataDxfId="17">
       <calculatedColumnFormula>AVERAGE(data!B4:D4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B852AE10-ECA0-4350-930A-0053985AAA92}" name="summer" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{B852AE10-ECA0-4350-930A-0053985AAA92}" name="summer" dataDxfId="16">
       <calculatedColumnFormula>AVERAGE(data!E4:G4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -372,13 +305,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D57E308-665D-4038-9E21-FE617E5E3EA4}" name="Tableau14" displayName="Tableau14" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{7D57E308-665D-4038-9E21-FE617E5E3EA4}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C57A926C-2C28-4B19-A5ED-17AF97673E7A}" name="time" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{C57A926C-2C28-4B19-A5ED-17AF97673E7A}" name="time" dataDxfId="15">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FA65F6A0-665C-4405-A62B-12823208AD5D}" name="winter" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{FA65F6A0-665C-4405-A62B-12823208AD5D}" name="winter" dataDxfId="14">
       <calculatedColumnFormula>AVERAGE(data!I4:K4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1C61CFA1-D2EF-4BD5-B9B4-B38B5F605685}" name="summer" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{1C61CFA1-D2EF-4BD5-B9B4-B38B5F605685}" name="summer" dataDxfId="13">
       <calculatedColumnFormula>AVERAGE(data!L4:N4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -390,13 +323,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BC8C08E7-0110-4508-8861-EEC92D3C6030}" name="Tableau15" displayName="Tableau15" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{BC8C08E7-0110-4508-8861-EEC92D3C6030}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAA9E51A-5AD7-4867-9998-9A02D34F9A4F}" name="time" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{AAA9E51A-5AD7-4867-9998-9A02D34F9A4F}" name="time" dataDxfId="12">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2C723683-0559-41C2-B136-D72947194399}" name="winter" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{2C723683-0559-41C2-B136-D72947194399}" name="winter" dataDxfId="11">
       <calculatedColumnFormula>AVERAGE(data!W4:Y4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{048BEDDA-CEBF-44D1-94E2-018176489471}" name="summer" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{048BEDDA-CEBF-44D1-94E2-018176489471}" name="summer" dataDxfId="7">
       <calculatedColumnFormula>AVERAGE(data!Z4:AB4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -408,15 +341,37 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F83A73E2-5F97-4D71-BEEA-A69C66F729DA}" name="Tableau16" displayName="Tableau16" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{F83A73E2-5F97-4D71-BEEA-A69C66F729DA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6152D57E-22A4-4756-83FF-0FA2A5A8826C}" name="time" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{6152D57E-22A4-4756-83FF-0FA2A5A8826C}" name="time" dataDxfId="10">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{03763A0D-A48C-4D52-886F-3E4E1070B03F}" name="winter" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{03763A0D-A48C-4D52-886F-3E4E1070B03F}" name="winter" dataDxfId="9">
       <calculatedColumnFormula>AVERAGE(data!P4:R4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{71CCAC2C-5701-474F-9EC1-E2F89CC65AAC}" name="summer" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{71CCAC2C-5701-474F-9EC1-E2F89CC65AAC}" name="summer" dataDxfId="8">
       <calculatedColumnFormula>AVERAGE(data!S4:U4)</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{65500618-7955-4477-BB55-B536E81F0228}" name="Tableau6" displayName="Tableau6" ref="A1:E97" totalsRowShown="0" headerRowDxfId="6" dataDxfId="2">
+  <autoFilter ref="A1:E97" xr:uid="{65500618-7955-4477-BB55-B536E81F0228}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0961E0D0-891A-498A-A97C-97FD88EDA497}" name="Courbe N1 winter" dataDxfId="5">
+      <calculatedColumnFormula>Tableau14[[#This Row],[winter]]*tests!$G$5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{E7E512C2-6011-4E3C-843A-EB7AFE4B64D0}" name="Courbe N1 winter avec valeur normalisée" dataDxfId="4">
+      <calculatedColumnFormula>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{60EA1D1C-592A-452F-8891-9A2A53F3EFED}" name="Courbe 55 summer" dataDxfId="0">
+      <calculatedColumnFormula>Tableau1[[#This Row],[summer]]*$M$27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{6BF445AF-DBBF-42AC-8A36-DAEF4B510253}" name="Courbe 55 summer avec valeur normalisée" dataDxfId="1">
+      <calculatedColumnFormula>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{46E29576-C0F4-498B-BC37-5C2F6F037758}" name="Courbe N5" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -687,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C97"/>
     </sheetView>
   </sheetViews>
@@ -4810,15 +4765,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E8C573-3C8F-437A-8FD2-727839301987}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -4829,7 +4784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>data!A4</f>
         <v>1.0416666666666666E-2</v>
@@ -4842,8 +4797,10 @@
         <f>AVERAGE(data!Z4:AB4)</f>
         <v>67.466666666666654</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>data!A5</f>
         <v>2.0833333333333332E-2</v>
@@ -4856,8 +4813,10 @@
         <f>AVERAGE(data!Z5:AB5)</f>
         <v>63.466666666666669</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>data!A6</f>
         <v>3.125E-2</v>
@@ -4870,8 +4829,10 @@
         <f>AVERAGE(data!Z6:AB6)</f>
         <v>60.333333333333336</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>data!A7</f>
         <v>4.1666666666666664E-2</v>
@@ -4884,8 +4845,12 @@
         <f>AVERAGE(data!Z7:AB7)</f>
         <v>57.733333333333327</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>data!A8</f>
         <v>5.2083333333333336E-2</v>
@@ -4898,8 +4863,10 @@
         <f>AVERAGE(data!Z8:AB8)</f>
         <v>55.300000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>data!A9</f>
         <v>6.25E-2</v>
@@ -4912,8 +4879,10 @@
         <f>AVERAGE(data!Z9:AB9)</f>
         <v>53.033333333333331</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>data!A10</f>
         <v>7.2916666666666671E-2</v>
@@ -4926,8 +4895,10 @@
         <f>AVERAGE(data!Z10:AB10)</f>
         <v>50.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>data!A11</f>
         <v>8.3333333333333329E-2</v>
@@ -4940,8 +4911,12 @@
         <f>AVERAGE(data!Z11:AB11)</f>
         <v>48.866666666666667</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f>data!A12</f>
         <v>9.375E-2</v>
@@ -4954,8 +4929,10 @@
         <f>AVERAGE(data!Z12:AB12)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f>data!A13</f>
         <v>0.10416666666666667</v>
@@ -4968,8 +4945,10 @@
         <f>AVERAGE(data!Z13:AB13)</f>
         <v>45.333333333333336</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f>data!A14</f>
         <v>0.11458333333333333</v>
@@ -4982,8 +4961,10 @@
         <f>AVERAGE(data!Z14:AB14)</f>
         <v>43.866666666666667</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>data!A15</f>
         <v>0.125</v>
@@ -4996,8 +4977,10 @@
         <f>AVERAGE(data!Z15:AB15)</f>
         <v>42.733333333333327</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>data!A16</f>
         <v>0.13541666666666666</v>
@@ -5010,8 +4993,10 @@
         <f>AVERAGE(data!Z16:AB16)</f>
         <v>41.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f>data!A17</f>
         <v>0.14583333333333334</v>
@@ -5024,8 +5009,10 @@
         <f>AVERAGE(data!Z17:AB17)</f>
         <v>41.300000000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f>data!A18</f>
         <v>0.15625</v>
@@ -5038,8 +5025,10 @@
         <f>AVERAGE(data!Z18:AB18)</f>
         <v>40.733333333333334</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f>data!A19</f>
         <v>0.16666666666666666</v>
@@ -5052,8 +5041,10 @@
         <f>AVERAGE(data!Z19:AB19)</f>
         <v>40.033333333333331</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f>data!A20</f>
         <v>0.17708333333333334</v>
@@ -5066,8 +5057,10 @@
         <f>AVERAGE(data!Z20:AB20)</f>
         <v>39.166666666666671</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f>data!A21</f>
         <v>0.1875</v>
@@ -5080,8 +5073,10 @@
         <f>AVERAGE(data!Z21:AB21)</f>
         <v>38.233333333333334</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f>data!A22</f>
         <v>0.19791666666666666</v>
@@ -5094,8 +5089,10 @@
         <f>AVERAGE(data!Z22:AB22)</f>
         <v>37.56666666666667</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f>data!A23</f>
         <v>0.20833333333333334</v>
@@ -5108,8 +5105,10 @@
         <f>AVERAGE(data!Z23:AB23)</f>
         <v>37.366666666666667</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f>data!A24</f>
         <v>0.21875</v>
@@ -5122,8 +5121,10 @@
         <f>AVERAGE(data!Z24:AB24)</f>
         <v>37.766666666666673</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f>data!A25</f>
         <v>0.22916666666666666</v>
@@ -5136,8 +5137,10 @@
         <f>AVERAGE(data!Z25:AB25)</f>
         <v>38.533333333333331</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f>data!A26</f>
         <v>0.23958333333333334</v>
@@ -5150,8 +5153,10 @@
         <f>AVERAGE(data!Z26:AB26)</f>
         <v>39.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f>data!A27</f>
         <v>0.25</v>
@@ -5164,8 +5169,10 @@
         <f>AVERAGE(data!Z27:AB27)</f>
         <v>40.033333333333331</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f>data!A28</f>
         <v>0.26041666666666669</v>
@@ -5178,8 +5185,10 @@
         <f>AVERAGE(data!Z28:AB28)</f>
         <v>40.233333333333334</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f>data!A29</f>
         <v>0.27083333333333331</v>
@@ -5192,8 +5201,10 @@
         <f>AVERAGE(data!Z29:AB29)</f>
         <v>40.333333333333336</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f>data!A30</f>
         <v>0.28125</v>
@@ -5206,8 +5217,10 @@
         <f>AVERAGE(data!Z30:AB30)</f>
         <v>41.033333333333331</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f>data!A31</f>
         <v>0.29166666666666669</v>
@@ -5220,8 +5233,10 @@
         <f>AVERAGE(data!Z31:AB31)</f>
         <v>42.733333333333327</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f>data!A32</f>
         <v>0.30208333333333331</v>
@@ -5234,8 +5249,10 @@
         <f>AVERAGE(data!Z32:AB32)</f>
         <v>45.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f>data!A33</f>
         <v>0.3125</v>
@@ -5248,8 +5265,10 @@
         <f>AVERAGE(data!Z33:AB33)</f>
         <v>50.266666666666673</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f>data!A34</f>
         <v>0.32291666666666669</v>
@@ -5262,8 +5281,10 @@
         <f>AVERAGE(data!Z34:AB34)</f>
         <v>55.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f>data!A35</f>
         <v>0.33333333333333331</v>
@@ -5276,8 +5297,10 @@
         <f>AVERAGE(data!Z35:AB35)</f>
         <v>60.800000000000004</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f>data!A36</f>
         <v>0.34375</v>
@@ -5290,8 +5313,10 @@
         <f>AVERAGE(data!Z36:AB36)</f>
         <v>66.266666666666666</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f>data!A37</f>
         <v>0.35416666666666669</v>
@@ -5304,8 +5329,10 @@
         <f>AVERAGE(data!Z37:AB37)</f>
         <v>71.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f>data!A38</f>
         <v>0.36458333333333331</v>
@@ -5318,8 +5345,10 @@
         <f>AVERAGE(data!Z38:AB38)</f>
         <v>77.166666666666671</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f>data!A39</f>
         <v>0.375</v>
@@ -5332,8 +5361,10 @@
         <f>AVERAGE(data!Z39:AB39)</f>
         <v>82.766666666666666</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f>data!A40</f>
         <v>0.38541666666666669</v>
@@ -5346,8 +5377,10 @@
         <f>AVERAGE(data!Z40:AB40)</f>
         <v>88.63333333333334</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f>data!A41</f>
         <v>0.39583333333333331</v>
@@ -5360,8 +5393,10 @@
         <f>AVERAGE(data!Z41:AB41)</f>
         <v>95.100000000000009</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f>data!A42</f>
         <v>0.40625</v>
@@ -5374,8 +5409,10 @@
         <f>AVERAGE(data!Z42:AB42)</f>
         <v>102.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f>data!A43</f>
         <v>0.41666666666666669</v>
@@ -5388,8 +5425,10 @@
         <f>AVERAGE(data!Z43:AB43)</f>
         <v>111.23333333333333</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f>data!A44</f>
         <v>0.42708333333333331</v>
@@ -5402,8 +5441,10 @@
         <f>AVERAGE(data!Z44:AB44)</f>
         <v>121.46666666666665</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f>data!A45</f>
         <v>0.4375</v>
@@ -5416,8 +5457,10 @@
         <f>AVERAGE(data!Z45:AB45)</f>
         <v>132.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f>data!A46</f>
         <v>0.44791666666666669</v>
@@ -5430,8 +5473,10 @@
         <f>AVERAGE(data!Z46:AB46)</f>
         <v>143.23333333333332</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f>data!A47</f>
         <v>0.45833333333333331</v>
@@ -5444,8 +5489,10 @@
         <f>AVERAGE(data!Z47:AB47)</f>
         <v>152.83333333333334</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f>data!A48</f>
         <v>0.46875</v>
@@ -5458,8 +5505,10 @@
         <f>AVERAGE(data!Z48:AB48)</f>
         <v>160.43333333333331</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f>data!A49</f>
         <v>0.47916666666666669</v>
@@ -5472,8 +5521,10 @@
         <f>AVERAGE(data!Z49:AB49)</f>
         <v>166.03333333333333</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f>data!A50</f>
         <v>0.48958333333333331</v>
@@ -5486,8 +5537,10 @@
         <f>AVERAGE(data!Z50:AB50)</f>
         <v>169.9</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f>data!A51</f>
         <v>0.5</v>
@@ -5500,8 +5553,10 @@
         <f>AVERAGE(data!Z51:AB51)</f>
         <v>172.06666666666669</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f>data!A52</f>
         <v>0.51041666666666663</v>
@@ -5514,8 +5569,10 @@
         <f>AVERAGE(data!Z52:AB52)</f>
         <v>172.79999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f>data!A53</f>
         <v>0.52083333333333337</v>
@@ -5528,8 +5585,10 @@
         <f>AVERAGE(data!Z53:AB53)</f>
         <v>172.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f>data!A54</f>
         <v>0.53125</v>
@@ -5542,8 +5601,10 @@
         <f>AVERAGE(data!Z54:AB54)</f>
         <v>171.46666666666667</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f>data!A55</f>
         <v>0.54166666666666663</v>
@@ -5556,8 +5617,10 @@
         <f>AVERAGE(data!Z55:AB55)</f>
         <v>170.1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f>data!A56</f>
         <v>0.55208333333333337</v>
@@ -5570,8 +5633,10 @@
         <f>AVERAGE(data!Z56:AB56)</f>
         <v>168.70000000000002</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f>data!A57</f>
         <v>0.5625</v>
@@ -5584,8 +5649,10 @@
         <f>AVERAGE(data!Z57:AB57)</f>
         <v>166.99999999999997</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f>data!A58</f>
         <v>0.57291666666666663</v>
@@ -5598,8 +5665,10 @@
         <f>AVERAGE(data!Z58:AB58)</f>
         <v>164.66666666666666</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f>data!A59</f>
         <v>0.58333333333333337</v>
@@ -5612,8 +5681,10 @@
         <f>AVERAGE(data!Z59:AB59)</f>
         <v>161.26666666666668</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f>data!A60</f>
         <v>0.59375</v>
@@ -5626,8 +5697,10 @@
         <f>AVERAGE(data!Z60:AB60)</f>
         <v>156.73333333333332</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f>data!A61</f>
         <v>0.60416666666666663</v>
@@ -5640,8 +5713,10 @@
         <f>AVERAGE(data!Z61:AB61)</f>
         <v>151.63333333333335</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f>data!A62</f>
         <v>0.61458333333333337</v>
@@ -5654,8 +5729,10 @@
         <f>AVERAGE(data!Z62:AB62)</f>
         <v>146.73333333333332</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f>data!A63</f>
         <v>0.625</v>
@@ -5668,8 +5745,10 @@
         <f>AVERAGE(data!Z63:AB63)</f>
         <v>142.80000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f>data!A64</f>
         <v>0.63541666666666663</v>
@@ -5682,8 +5761,10 @@
         <f>AVERAGE(data!Z64:AB64)</f>
         <v>140.43333333333331</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f>data!A65</f>
         <v>0.64583333333333337</v>
@@ -5696,8 +5777,10 @@
         <f>AVERAGE(data!Z65:AB65)</f>
         <v>139.23333333333332</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f>data!A66</f>
         <v>0.65625</v>
@@ -5710,8 +5793,10 @@
         <f>AVERAGE(data!Z66:AB66)</f>
         <v>138.56666666666666</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <f>data!A67</f>
         <v>0.66666666666666663</v>
@@ -5724,8 +5809,10 @@
         <f>AVERAGE(data!Z67:AB67)</f>
         <v>137.83333333333334</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <f>data!A68</f>
         <v>0.67708333333333337</v>
@@ -5738,8 +5825,10 @@
         <f>AVERAGE(data!Z68:AB68)</f>
         <v>136.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <f>data!A69</f>
         <v>0.6875</v>
@@ -5752,8 +5841,10 @@
         <f>AVERAGE(data!Z69:AB69)</f>
         <v>135.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <f>data!A70</f>
         <v>0.69791666666666663</v>
@@ -5766,8 +5857,10 @@
         <f>AVERAGE(data!Z70:AB70)</f>
         <v>135.33333333333334</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <f>data!A71</f>
         <v>0.70833333333333337</v>
@@ -5780,8 +5873,10 @@
         <f>AVERAGE(data!Z71:AB71)</f>
         <v>137.03333333333333</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f>data!A72</f>
         <v>0.71875</v>
@@ -5794,8 +5889,10 @@
         <f>AVERAGE(data!Z72:AB72)</f>
         <v>141.13333333333333</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <f>data!A73</f>
         <v>0.72916666666666663</v>
@@ -5808,8 +5905,10 @@
         <f>AVERAGE(data!Z73:AB73)</f>
         <v>147.23333333333332</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <f>data!A74</f>
         <v>0.73958333333333337</v>
@@ -5822,8 +5921,10 @@
         <f>AVERAGE(data!Z74:AB74)</f>
         <v>154.79999999999998</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <f>data!A75</f>
         <v>0.75</v>
@@ -5836,8 +5937,10 @@
         <f>AVERAGE(data!Z75:AB75)</f>
         <v>163.20000000000002</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <f>data!A76</f>
         <v>0.76041666666666663</v>
@@ -5850,8 +5953,10 @@
         <f>AVERAGE(data!Z76:AB76)</f>
         <v>171.86666666666665</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <f>data!A77</f>
         <v>0.77083333333333337</v>
@@ -5864,8 +5969,10 @@
         <f>AVERAGE(data!Z77:AB77)</f>
         <v>180.20000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <f>data!A78</f>
         <v>0.78125</v>
@@ -5878,8 +5985,10 @@
         <f>AVERAGE(data!Z78:AB78)</f>
         <v>187.63333333333333</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <f>data!A79</f>
         <v>0.79166666666666663</v>
@@ -5892,8 +6001,10 @@
         <f>AVERAGE(data!Z79:AB79)</f>
         <v>193.6</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <f>data!A80</f>
         <v>0.80208333333333337</v>
@@ -5906,8 +6017,10 @@
         <f>AVERAGE(data!Z80:AB80)</f>
         <v>197.76666666666665</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <f>data!A81</f>
         <v>0.8125</v>
@@ -5920,8 +6033,10 @@
         <f>AVERAGE(data!Z81:AB81)</f>
         <v>200.19999999999996</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <f>data!A82</f>
         <v>0.82291666666666663</v>
@@ -5934,8 +6049,10 @@
         <f>AVERAGE(data!Z82:AB82)</f>
         <v>201.16666666666666</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <f>data!A83</f>
         <v>0.83333333333333337</v>
@@ -5948,8 +6065,10 @@
         <f>AVERAGE(data!Z83:AB83)</f>
         <v>200.93333333333331</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <f>data!A84</f>
         <v>0.84375</v>
@@ -5962,8 +6081,10 @@
         <f>AVERAGE(data!Z84:AB84)</f>
         <v>199.73333333333335</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <f>data!A85</f>
         <v>0.85416666666666663</v>
@@ -5976,8 +6097,10 @@
         <f>AVERAGE(data!Z85:AB85)</f>
         <v>197.6</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <f>data!A86</f>
         <v>0.86458333333333337</v>
@@ -5990,8 +6113,10 @@
         <f>AVERAGE(data!Z86:AB86)</f>
         <v>194.53333333333333</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <f>data!A87</f>
         <v>0.875</v>
@@ -6004,8 +6129,10 @@
         <f>AVERAGE(data!Z87:AB87)</f>
         <v>190.56666666666669</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <f>data!A88</f>
         <v>0.88541666666666663</v>
@@ -6018,8 +6145,10 @@
         <f>AVERAGE(data!Z88:AB88)</f>
         <v>185.5333333333333</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <f>data!A89</f>
         <v>0.89583333333333337</v>
@@ -6032,8 +6161,10 @@
         <f>AVERAGE(data!Z89:AB89)</f>
         <v>179.36666666666667</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <f>data!A90</f>
         <v>0.90625</v>
@@ -6046,8 +6177,10 @@
         <f>AVERAGE(data!Z90:AB90)</f>
         <v>171.83333333333334</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <f>data!A91</f>
         <v>0.91666666666666663</v>
@@ -6060,8 +6193,10 @@
         <f>AVERAGE(data!Z91:AB91)</f>
         <v>162.83333333333331</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <f>data!A92</f>
         <v>0.92708333333333337</v>
@@ -6074,8 +6209,10 @@
         <f>AVERAGE(data!Z92:AB92)</f>
         <v>152.19999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <f>data!A93</f>
         <v>0.9375</v>
@@ -6088,8 +6225,10 @@
         <f>AVERAGE(data!Z93:AB93)</f>
         <v>140.33333333333331</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <f>data!A94</f>
         <v>0.94791666666666663</v>
@@ -6102,8 +6241,10 @@
         <f>AVERAGE(data!Z94:AB94)</f>
         <v>127.93333333333332</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <f>data!A95</f>
         <v>0.95833333333333337</v>
@@ -6116,8 +6257,10 @@
         <f>AVERAGE(data!Z95:AB95)</f>
         <v>115.46666666666665</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <f>data!A96</f>
         <v>0.96875</v>
@@ -6130,8 +6273,10 @@
         <f>AVERAGE(data!Z96:AB96)</f>
         <v>103.5</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <f>data!A97</f>
         <v>0.97916666666666663</v>
@@ -6144,8 +6289,10 @@
         <f>AVERAGE(data!Z97:AB97)</f>
         <v>92.333333333333329</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <f>data!A98</f>
         <v>0.98958333333333337</v>
@@ -6158,8 +6305,10 @@
         <f>AVERAGE(data!Z98:AB98)</f>
         <v>82.233333333333334</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <f>data!A99</f>
         <v>0</v>
@@ -6172,8 +6321,11 @@
         <f>AVERAGE(data!Z99:AB99)</f>
         <v>73.533333333333331</v>
       </c>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -15415,4 +15567,1909 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59B84D5-23AE-443A-9387-1164FF364677}">
+  <dimension ref="A1:M97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1240.2163199999998</v>
+      </c>
+      <c r="B2" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1152.0163186230973</v>
+      </c>
+      <c r="C2" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2272.4078800000002</v>
+      </c>
+      <c r="D2" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2146.5784054196097</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1204.38528</v>
+      </c>
+      <c r="B3" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1118.7334613283015</v>
+      </c>
+      <c r="C3" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2092.2278200000001</v>
+      </c>
+      <c r="D3" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1976.3754109276128</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1177.8009599999998</v>
+      </c>
+      <c r="B4" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1094.0397284966787</v>
+      </c>
+      <c r="C4" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1936.7299600000006</v>
+      </c>
+      <c r="D4" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1829.4878951331507</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1156.4179199999999</v>
+      </c>
+      <c r="B5" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1074.1773781755908</v>
+      </c>
+      <c r="C5" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1800.9778600000002</v>
+      </c>
+      <c r="D5" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1701.2527622967145</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3">
+        <v>17.337599999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1137.34656</v>
+      </c>
+      <c r="B6" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1056.4623089702961</v>
+      </c>
+      <c r="C6" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1676.7441200000003</v>
+      </c>
+      <c r="D6" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1583.8981861857947</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1119.4310400000002</v>
+      </c>
+      <c r="B7" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1039.8208803228983</v>
+      </c>
+      <c r="C7" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1568.1424400000003</v>
+      </c>
+      <c r="D7" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1481.3100799166459</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1103.2492799999998</v>
+      </c>
+      <c r="B8" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1024.7899125123452</v>
+      </c>
+      <c r="C8" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1473.5273400000001</v>
+      </c>
+      <c r="D8" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1391.9340782427664</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1086.4895999999999</v>
+      </c>
+      <c r="B9" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1009.2221244228439</v>
+      </c>
+      <c r="C9" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1396.1897799999999</v>
+      </c>
+      <c r="D9" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1318.8789116571604</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1070.8857599999999</v>
+      </c>
+      <c r="B10" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>994.72797689123922</v>
+      </c>
+      <c r="C10" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1339.4207200000003</v>
+      </c>
+      <c r="D10" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1265.2533106528331</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="H10">
+        <f>SUM(Tableau6[Courbe N1 winter avec valeur normalisée])*365*0.25/1000</f>
+        <v>17337.599999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1056.43776</v>
+      </c>
+      <c r="B11" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>981.30746991753131</v>
+      </c>
+      <c r="C11" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1299.10646</v>
+      </c>
+      <c r="D11" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1227.1713621135275</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1041.4118399999998</v>
+      </c>
+      <c r="B12" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>967.35014266487474</v>
+      </c>
+      <c r="C12" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1267.8423400000004</v>
+      </c>
+      <c r="D12" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1197.6384224299852</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1028.11968</v>
+      </c>
+      <c r="B13" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>955.00327624906356</v>
+      </c>
+      <c r="C13" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1246.4511</v>
+      </c>
+      <c r="D13" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1177.4316742254555</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="G13">
+        <f>SUM(Tableau14[winter])*365*0.25/1000</f>
+        <v>1076.5614166666669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1014.8275199999998</v>
+      </c>
+      <c r="B14" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>942.65640983325193</v>
+      </c>
+      <c r="C14" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1228.3508200000003</v>
+      </c>
+      <c r="D14" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1160.3336565139311</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1002.6912</v>
+      </c>
+      <c r="B15" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>931.38318397533737</v>
+      </c>
+      <c r="C15" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1215.1869799999999</v>
+      </c>
+      <c r="D15" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1147.8987345419127</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>992.86656000000005</v>
+      </c>
+      <c r="B16" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>922.25723923321596</v>
+      </c>
+      <c r="C16" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1206.1368400000001</v>
+      </c>
+      <c r="D16" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1139.3497256861506</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>984.77567999999997</v>
+      </c>
+      <c r="B17" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>914.74175532793936</v>
+      </c>
+      <c r="C17" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1204.4913600000002</v>
+      </c>
+      <c r="D17" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1137.7953604396484</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>980.15231999999992</v>
+      </c>
+      <c r="B18" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>910.44719309635275</v>
+      </c>
+      <c r="C18" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1210.25054</v>
+      </c>
+      <c r="D18" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1143.2356388024061</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>980.15231999999992</v>
+      </c>
+      <c r="B19" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>910.44719309635275</v>
+      </c>
+      <c r="C19" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1220.9461600000002</v>
+      </c>
+      <c r="D19" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1153.3390129046709</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>984.77567999999997</v>
+      </c>
+      <c r="B20" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>914.74175532793936</v>
+      </c>
+      <c r="C20" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1234.9327400000002</v>
+      </c>
+      <c r="D20" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1166.5511174999399</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>995.17823999999985</v>
+      </c>
+      <c r="B21" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>924.40452034900909</v>
+      </c>
+      <c r="C21" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1246.4511</v>
+      </c>
+      <c r="D21" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1177.4316742254555</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1014.2495999999999</v>
+      </c>
+      <c r="B22" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>942.11958955430373</v>
+      </c>
+      <c r="C22" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1258.7922000000001</v>
+      </c>
+      <c r="D22" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1189.0894135742226</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1043.7235199999998</v>
+      </c>
+      <c r="B23" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>969.49742378066799</v>
+      </c>
+      <c r="C23" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1278.5379600000001</v>
+      </c>
+      <c r="D23" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1207.7417965322495</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1086.4895999999999</v>
+      </c>
+      <c r="B24" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1009.2221244228439</v>
+      </c>
+      <c r="C24" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1320.4977000000001</v>
+      </c>
+      <c r="D24" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1247.378110318057</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1145.4374399999999</v>
+      </c>
+      <c r="B25" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1063.9777928755727</v>
+      </c>
+      <c r="C25" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1397.0125200000002</v>
+      </c>
+      <c r="D25" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1319.6560942804117</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1224.6124799999998</v>
+      </c>
+      <c r="B26" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1137.5221710914925</v>
+      </c>
+      <c r="C26" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1514.6643400000003</v>
+      </c>
+      <c r="D26" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1430.7932094053228</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="M26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1332.1055999999999</v>
+      </c>
+      <c r="B27" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1237.3707429758804</v>
+      </c>
+      <c r="C27" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1663.5802799999999</v>
+      </c>
+      <c r="D27" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1571.4632642137763</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="M27">
+        <f>(4618.2+7546+12518)/1000</f>
+        <v>24.682200000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1476.0076799999997</v>
+      </c>
+      <c r="B28" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1371.0389924340122</v>
+      </c>
+      <c r="C28" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1829.77376</v>
+      </c>
+      <c r="D28" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1728.4541541105039</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1664.4096</v>
+      </c>
+      <c r="B29" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1546.0424033711652</v>
+      </c>
+      <c r="C29" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>1999.2582000000002</v>
+      </c>
+      <c r="D29" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>1888.5537745002359</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="M29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1903.6684799999998</v>
+      </c>
+      <c r="B30" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1768.28599885577</v>
+      </c>
+      <c r="C30" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2161.3379800000002</v>
+      </c>
+      <c r="D30" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2041.6587512807077</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="M30">
+        <f>SUM(Tableau1[summer])*365*0.25/1000</f>
+        <v>1058.6186250000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2182.80384</v>
+      </c>
+      <c r="B31" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2027.5701935878094</v>
+      </c>
+      <c r="C31" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2320.1268</v>
+      </c>
+      <c r="D31" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2191.6549975681746</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2489.6793599999996</v>
+      </c>
+      <c r="B32" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2312.6217617093675</v>
+      </c>
+      <c r="C32" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2482.20658</v>
+      </c>
+      <c r="D32" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2344.7599743486467</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="M32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2810.4249599999998</v>
+      </c>
+      <c r="B33" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2610.5570165256863</v>
+      </c>
+      <c r="C33" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2656.6274600000002</v>
+      </c>
+      <c r="D33" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2509.5226904778851</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="M33">
+        <f>SUM(Tableau6[Courbe 55 summer avec valeur normalisée])*365*0.25/1000</f>
+        <v>24682.199999999986</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3128.2809599999991</v>
+      </c>
+      <c r="B34" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2905.8081699472623</v>
+      </c>
+      <c r="C34" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2849.1486200000004</v>
+      </c>
+      <c r="D34" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2691.3834243186488</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3417.2409599999996</v>
+      </c>
+      <c r="B35" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3174.2183094214233</v>
+      </c>
+      <c r="C35" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3049.8971799999999</v>
+      </c>
+      <c r="D35" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2881.0159843919232</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3644.3635199999999</v>
+      </c>
+      <c r="B36" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3385.188679048114</v>
+      </c>
+      <c r="C36" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3249.8229999999999</v>
+      </c>
+      <c r="D36" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3069.8713618419465</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3779.5967999999998</v>
+      </c>
+      <c r="B37" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3510.804624322021</v>
+      </c>
+      <c r="C37" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3437.4077200000006</v>
+      </c>
+      <c r="D37" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3247.0689999432043</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3801.5577599999992</v>
+      </c>
+      <c r="B38" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3531.2037949220567</v>
+      </c>
+      <c r="C38" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3602.7784600000005</v>
+      </c>
+      <c r="D38" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3403.2827072166801</v>
+      </c>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3726.428159999999</v>
+      </c>
+      <c r="B39" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3461.4171586587745</v>
+      </c>
+      <c r="C39" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3744.2897400000006</v>
+      </c>
+      <c r="D39" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3536.9581184158742</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3580.2143999999998</v>
+      </c>
+      <c r="B40" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3325.6016280848503</v>
+      </c>
+      <c r="C40" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3856.1823799999997</v>
+      </c>
+      <c r="D40" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3642.6549551780263</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3388.3449599999994</v>
+      </c>
+      <c r="B41" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3147.377295474007</v>
+      </c>
+      <c r="C41" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3937.63364</v>
+      </c>
+      <c r="D41" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3719.5960348798881</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3177.4041599999996</v>
+      </c>
+      <c r="B42" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2951.4378936578701</v>
+      </c>
+      <c r="C42" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3989.4662600000006</v>
+      </c>
+      <c r="D42" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3768.5585401447092</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2978.5996799999994</v>
+      </c>
+      <c r="B43" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2766.7717176996471</v>
+      </c>
+      <c r="C43" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4021.5531199999996</v>
+      </c>
+      <c r="D43" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3798.8686624515026</v>
+      </c>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2820.2495999999996</v>
+      </c>
+      <c r="B44" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2619.6829612678075</v>
+      </c>
+      <c r="C44" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4049.52628</v>
+      </c>
+      <c r="D44" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3825.2928716420411</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2735.8732799999993</v>
+      </c>
+      <c r="B45" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2541.3072005413524</v>
+      </c>
+      <c r="C45" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4088.19506</v>
+      </c>
+      <c r="D45" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3861.8204549348438</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2740.4966399999998</v>
+      </c>
+      <c r="B46" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2545.6017627729393</v>
+      </c>
+      <c r="C46" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4146.6096000000007</v>
+      </c>
+      <c r="D46" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3917.0004211856744</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2794.8211200000001</v>
+      </c>
+      <c r="B47" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2596.0628689940818</v>
+      </c>
+      <c r="C47" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4222.3016800000005</v>
+      </c>
+      <c r="D47" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3988.5012225247779</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2845.6780799999997</v>
+      </c>
+      <c r="B48" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2643.3030535415337</v>
+      </c>
+      <c r="C48" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4308.6893800000007</v>
+      </c>
+      <c r="D48" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4070.1053979661465</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2837.5871999999995</v>
+      </c>
+      <c r="B49" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2635.7875696362571</v>
+      </c>
+      <c r="C49" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4395.8998200000005</v>
+      </c>
+      <c r="D49" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4152.4867560307657</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2732.4057599999996</v>
+      </c>
+      <c r="B50" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2538.0862788676627</v>
+      </c>
+      <c r="C50" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4477.3510800000004</v>
+      </c>
+      <c r="D50" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4229.4278357326266</v>
+      </c>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2560.7635199999995</v>
+      </c>
+      <c r="B51" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2378.650656020011</v>
+      </c>
+      <c r="C51" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4536.5883600000016</v>
+      </c>
+      <c r="D51" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4285.3849846067087</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2364.2707199999995</v>
+      </c>
+      <c r="B52" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2196.1317611775817</v>
+      </c>
+      <c r="C52" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4553.0431600000002</v>
+      </c>
+      <c r="D52" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4300.92863707173</v>
+      </c>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2189.1609599999997</v>
+      </c>
+      <c r="B53" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2033.4752166562407</v>
+      </c>
+      <c r="C53" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4512.728900000001</v>
+      </c>
+      <c r="D53" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4262.846688532426</v>
+      </c>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2068.9535999999998</v>
+      </c>
+      <c r="B54" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1921.81659863499</v>
+      </c>
+      <c r="C54" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4401.6590000000006</v>
+      </c>
+      <c r="D54" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4157.9270343935232</v>
+      </c>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1996.7135999999998</v>
+      </c>
+      <c r="B55" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1854.7140637664497</v>
+      </c>
+      <c r="C55" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4242.8701800000008</v>
+      </c>
+      <c r="D55" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>4007.9307881060563</v>
+      </c>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1953.3696</v>
+      </c>
+      <c r="B56" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1814.4525428453258</v>
+      </c>
+      <c r="C56" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4060.2218999999996</v>
+      </c>
+      <c r="D56" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3835.3962457443054</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1921.5839999999998</v>
+      </c>
+      <c r="B57" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1784.927427503168</v>
+      </c>
+      <c r="C57" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3883.3328000000006</v>
+      </c>
+      <c r="D57" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3668.3019817453142</v>
+      </c>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1886.9087999999997</v>
+      </c>
+      <c r="B58" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1752.7182107662686</v>
+      </c>
+      <c r="C58" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3731.1259</v>
+      </c>
+      <c r="D58" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3524.5231964438553</v>
+      </c>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1848.7660799999996</v>
+      </c>
+      <c r="B59" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1717.2880723556793</v>
+      </c>
+      <c r="C59" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3607.7148999999999</v>
+      </c>
+      <c r="D59" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3407.9458029561865</v>
+      </c>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1812.9350400000001</v>
+      </c>
+      <c r="B60" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1684.0052150608838</v>
+      </c>
+      <c r="C60" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3501.5814400000004</v>
+      </c>
+      <c r="D60" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3307.6892445567919</v>
+      </c>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1782.8831999999998</v>
+      </c>
+      <c r="B61" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1656.0905605555708</v>
+      </c>
+      <c r="C61" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3410.2573000000002</v>
+      </c>
+      <c r="D61" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3221.4219733759164</v>
+      </c>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1760.9222399999999</v>
+      </c>
+      <c r="B62" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1635.6913899555348</v>
+      </c>
+      <c r="C62" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3327.1605599999998</v>
+      </c>
+      <c r="D62" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3142.9265284275525</v>
+      </c>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1748.78592</v>
+      </c>
+      <c r="B63" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1624.4181640976201</v>
+      </c>
+      <c r="C63" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3251.4684800000005</v>
+      </c>
+      <c r="D63" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3071.4257270884495</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1745.3183999999999</v>
+      </c>
+      <c r="B64" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1621.19724242393</v>
+      </c>
+      <c r="C64" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3184.0038000000004</v>
+      </c>
+      <c r="D64" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3007.6967519818572</v>
+      </c>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1750.5196799999997</v>
+      </c>
+      <c r="B65" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1626.0286249344647</v>
+      </c>
+      <c r="C65" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3122.2983000000004</v>
+      </c>
+      <c r="D65" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2949.4080552380228</v>
+      </c>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1764.9676799999997</v>
+      </c>
+      <c r="B66" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1639.4491319081728</v>
+      </c>
+      <c r="C66" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3068.8202000000001</v>
+      </c>
+      <c r="D66" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2898.8911847266991</v>
+      </c>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1799.6428799999999</v>
+      </c>
+      <c r="B67" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1671.6583486450722</v>
+      </c>
+      <c r="C67" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3028.5059400000005</v>
+      </c>
+      <c r="D67" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2860.8092361873946</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1864.94784</v>
+      </c>
+      <c r="B68" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1732.3190401662328</v>
+      </c>
+      <c r="C68" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3006.29196</v>
+      </c>
+      <c r="D68" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2839.8253053596136</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1974.7526399999997</v>
+      </c>
+      <c r="B69" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1834.3148931664134</v>
+      </c>
+      <c r="C69" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3006.29196</v>
+      </c>
+      <c r="D69" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2839.8253053596136</v>
+      </c>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2137.7260799999999</v>
+      </c>
+      <c r="B70" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1985.6982118298404</v>
+      </c>
+      <c r="C70" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3032.6196400000003</v>
+      </c>
+      <c r="D70" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2864.6951493036499</v>
+      </c>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2347.5110399999999</v>
+      </c>
+      <c r="B71" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2180.5639730880807</v>
+      </c>
+      <c r="C71" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3084.4522600000005</v>
+      </c>
+      <c r="D71" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2913.6576545684711</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2596.5945599999995</v>
+      </c>
+      <c r="B72" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2411.933513314807</v>
+      </c>
+      <c r="C72" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3161.78982</v>
+      </c>
+      <c r="D72" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2986.7128211540762</v>
+      </c>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2874.5740799999994</v>
+      </c>
+      <c r="B73" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2670.1440674889495</v>
+      </c>
+      <c r="C73" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3259.6958800000002</v>
+      </c>
+      <c r="D73" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3079.1975533209607</v>
+      </c>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3171.0470399999999</v>
+      </c>
+      <c r="B74" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2945.5328705894385</v>
+      </c>
+      <c r="C74" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3375.7022200000006</v>
+      </c>
+      <c r="D74" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3188.7803031993694</v>
+      </c>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3461.7407999999996</v>
+      </c>
+      <c r="B75" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3215.5534709004442</v>
+      </c>
+      <c r="C75" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3507.3406199999999</v>
+      </c>
+      <c r="D75" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3313.1295229195493</v>
+      </c>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3719.4931199999996</v>
+      </c>
+      <c r="B76" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3454.9753153113952</v>
+      </c>
+      <c r="C76" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3648.8519000000006</v>
+      </c>
+      <c r="D76" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3446.8049341187434</v>
+      </c>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3918.2975999999994</v>
+      </c>
+      <c r="B77" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3639.6414912696177</v>
+      </c>
+      <c r="C77" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3794.4768799999997</v>
+      </c>
+      <c r="D77" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3584.3662584341919</v>
+      </c>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>4034.4595199999999</v>
+      </c>
+      <c r="B78" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3747.5423673382306</v>
+      </c>
+      <c r="C78" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3936.8109000000004</v>
+      </c>
+      <c r="D78" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3718.818852256637</v>
+      </c>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>4058.7321599999996</v>
+      </c>
+      <c r="B79" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3770.08881905406</v>
+      </c>
+      <c r="C79" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4065.1583400000009</v>
+      </c>
+      <c r="D79" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3840.0593414838131</v>
+      </c>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3983.6025599999994</v>
+      </c>
+      <c r="B80" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3700.3021827907778</v>
+      </c>
+      <c r="C80" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4161.4189200000001</v>
+      </c>
+      <c r="D80" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3930.9897084041941</v>
+      </c>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3806.1811199999997</v>
+      </c>
+      <c r="B81" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3535.4983571536436</v>
+      </c>
+      <c r="C81" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4210.7833200000005</v>
+      </c>
+      <c r="D81" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3977.620665799262</v>
+      </c>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3527.6236799999997</v>
+      </c>
+      <c r="B82" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>3276.7509827005529</v>
+      </c>
+      <c r="C82" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4205.0241400000004</v>
+      </c>
+      <c r="D82" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3972.1803874365041</v>
+      </c>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>3188.3846399999998</v>
+      </c>
+      <c r="B83" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2961.6374789578881</v>
+      </c>
+      <c r="C83" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4153.1915200000003</v>
+      </c>
+      <c r="D83" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3923.2178821716834</v>
+      </c>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2838.1651200000001</v>
+      </c>
+      <c r="B84" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2636.3243899152058</v>
+      </c>
+      <c r="C84" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>4075.0312200000003</v>
+      </c>
+      <c r="D84" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3849.3855329628263</v>
+      </c>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2526.66624</v>
+      </c>
+      <c r="B85" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2346.9782595620604</v>
+      </c>
+      <c r="C85" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3985.3525600000003</v>
+      </c>
+      <c r="D85" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3764.6726270284535</v>
+      </c>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2291.4527999999996</v>
+      </c>
+      <c r="B86" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>2128.4924060300932</v>
+      </c>
+      <c r="C86" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3900.6103400000002</v>
+      </c>
+      <c r="D86" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3684.6228168335874</v>
+      </c>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2123.8559999999998</v>
+      </c>
+      <c r="B87" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1972.8145251350804</v>
+      </c>
+      <c r="C87" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3825.7410000000004</v>
+      </c>
+      <c r="D87" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3613.8991981177351</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>2004.2265600000001</v>
+      </c>
+      <c r="B88" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1861.6927273927781</v>
+      </c>
+      <c r="C88" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3761.5672800000002</v>
+      </c>
+      <c r="D88" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3553.2789535041475</v>
+      </c>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1911.7593599999998</v>
+      </c>
+      <c r="B89" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1775.8014827610466</v>
+      </c>
+      <c r="C89" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3711.3801400000007</v>
+      </c>
+      <c r="D89" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3505.8708134858289</v>
+      </c>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1828.5388799999996</v>
+      </c>
+      <c r="B90" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1698.4993625924881</v>
+      </c>
+      <c r="C90" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3671.0658800000006</v>
+      </c>
+      <c r="D90" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3467.788864946524</v>
+      </c>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1748.7859199999998</v>
+      </c>
+      <c r="B91" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1624.4181640976199</v>
+      </c>
+      <c r="C91" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3624.1697000000004</v>
+      </c>
+      <c r="D91" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3423.4894554212092</v>
+      </c>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1671.3446399999998</v>
+      </c>
+      <c r="B92" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1552.4842467185449</v>
+      </c>
+      <c r="C92" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3546.8321400000009</v>
+      </c>
+      <c r="D92" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3350.4342888356041</v>
+      </c>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1589.8579199999999</v>
+      </c>
+      <c r="B93" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1476.7925873868317</v>
+      </c>
+      <c r="C93" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3417.6619600000004</v>
+      </c>
+      <c r="D93" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3228.4166169851769</v>
+      </c>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1504.3257599999995</v>
+      </c>
+      <c r="B94" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1397.3431861024799</v>
+      </c>
+      <c r="C94" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>3220.2043600000002</v>
+      </c>
+      <c r="D94" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>3041.8927874049064</v>
+      </c>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1418.7935999999997</v>
+      </c>
+      <c r="B95" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1317.8937848181286</v>
+      </c>
+      <c r="C95" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2975.0278400000007</v>
+      </c>
+      <c r="D95" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2810.2923656760713</v>
+      </c>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1338.46272</v>
+      </c>
+      <c r="B96" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1243.2757660443119</v>
+      </c>
+      <c r="C96" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2707.6373400000002</v>
+      </c>
+      <c r="D96" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2557.7080131194552</v>
+      </c>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <f>Tableau14[[#This Row],[winter]]*tests!$G$5</f>
+        <v>1269.11232</v>
+      </c>
+      <c r="B97" s="3">
+        <f>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</f>
+        <v>1178.8573325705133</v>
+      </c>
+      <c r="C97" s="3">
+        <f>Tableau1[[#This Row],[summer]]*$M$27</f>
+        <v>2444.3605400000006</v>
+      </c>
+      <c r="D97" s="3">
+        <f>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</f>
+        <v>2309.0095736790954</v>
+      </c>
+      <c r="E97" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding heat pump and industrial heat consumption
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/data/Load_curves.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/data/Load_curves.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micael\git\rhtlab_MIB\Mini-projet-trey_Buchser_Joye\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6700B8-803B-4235-9C41-37B7D695BE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1887BCD-88BC-4243-941E-3A2F3A90411A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="one_housing" sheetId="1" r:id="rId1"/>
     <sheet name="multi_housing" sheetId="3" r:id="rId2"/>
     <sheet name="farm" sheetId="4" r:id="rId3"/>
     <sheet name="church" sheetId="5" r:id="rId4"/>
-    <sheet name="industrial" sheetId="6" r:id="rId5"/>
+    <sheet name="industial" sheetId="6" r:id="rId5"/>
     <sheet name="data" sheetId="2" r:id="rId6"/>
     <sheet name="tests" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -185,35 +185,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="11"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -297,13 +269,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1423AFD3-B1FF-4ECC-97A3-6C69EC5E382E}" name="Tableau1" displayName="Tableau1" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{1423AFD3-B1FF-4ECC-97A3-6C69EC5E382E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F4A83B21-5B90-4E3A-A4C4-21CB26A32609}" name="time" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{F4A83B21-5B90-4E3A-A4C4-21CB26A32609}" name="time" dataDxfId="21">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9FC972AF-5398-4422-A201-4B4234DC1C8F}" name="winter" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{9FC972AF-5398-4422-A201-4B4234DC1C8F}" name="winter" dataDxfId="20">
       <calculatedColumnFormula>AVERAGE(data!B4:D4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{34FBB4B4-434F-4EEA-9B5E-62332F1AC62D}" name="summer" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{34FBB4B4-434F-4EEA-9B5E-62332F1AC62D}" name="summer" dataDxfId="19">
       <calculatedColumnFormula>AVERAGE(data!E4:G4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -315,13 +287,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3C8F13B-6B46-4563-B8EA-AC8CEE0E4FF4}" name="Tableau13" displayName="Tableau13" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{C3C8F13B-6B46-4563-B8EA-AC8CEE0E4FF4}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{792905A5-8492-44CE-BA07-2BE3F5926705}" name="time" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{792905A5-8492-44CE-BA07-2BE3F5926705}" name="time" dataDxfId="18">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{057D2796-C49B-4646-B908-BAB657B80C5A}" name="winter" dataDxfId="21">
+    <tableColumn id="2" xr3:uid="{057D2796-C49B-4646-B908-BAB657B80C5A}" name="winter" dataDxfId="17">
       <calculatedColumnFormula>AVERAGE(data!B4:D4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B852AE10-ECA0-4350-930A-0053985AAA92}" name="summer" dataDxfId="20">
+    <tableColumn id="3" xr3:uid="{B852AE10-ECA0-4350-930A-0053985AAA92}" name="summer" dataDxfId="16">
       <calculatedColumnFormula>AVERAGE(data!E4:G4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -333,13 +305,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D57E308-665D-4038-9E21-FE617E5E3EA4}" name="Tableau14" displayName="Tableau14" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{7D57E308-665D-4038-9E21-FE617E5E3EA4}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C57A926C-2C28-4B19-A5ED-17AF97673E7A}" name="time" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{C57A926C-2C28-4B19-A5ED-17AF97673E7A}" name="time" dataDxfId="15">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FA65F6A0-665C-4405-A62B-12823208AD5D}" name="winter" dataDxfId="18">
+    <tableColumn id="2" xr3:uid="{FA65F6A0-665C-4405-A62B-12823208AD5D}" name="winter" dataDxfId="14">
       <calculatedColumnFormula>AVERAGE(data!I4:K4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1C61CFA1-D2EF-4BD5-B9B4-B38B5F605685}" name="summer" dataDxfId="17">
+    <tableColumn id="3" xr3:uid="{1C61CFA1-D2EF-4BD5-B9B4-B38B5F605685}" name="summer" dataDxfId="13">
       <calculatedColumnFormula>AVERAGE(data!L4:N4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -351,13 +323,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BC8C08E7-0110-4508-8861-EEC92D3C6030}" name="Tableau15" displayName="Tableau15" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{BC8C08E7-0110-4508-8861-EEC92D3C6030}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAA9E51A-5AD7-4867-9998-9A02D34F9A4F}" name="time" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{AAA9E51A-5AD7-4867-9998-9A02D34F9A4F}" name="time" dataDxfId="12">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2C723683-0559-41C2-B136-D72947194399}" name="winter" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{2C723683-0559-41C2-B136-D72947194399}" name="winter" dataDxfId="11">
       <calculatedColumnFormula>AVERAGE(data!W4:Y4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{048BEDDA-CEBF-44D1-94E2-018176489471}" name="summer" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{048BEDDA-CEBF-44D1-94E2-018176489471}" name="summer" dataDxfId="10">
       <calculatedColumnFormula>AVERAGE(data!Z4:AB4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -369,13 +341,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F83A73E2-5F97-4D71-BEEA-A69C66F729DA}" name="Tableau16" displayName="Tableau16" ref="A1:C97" totalsRowShown="0">
   <autoFilter ref="A1:C97" xr:uid="{F83A73E2-5F97-4D71-BEEA-A69C66F729DA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6152D57E-22A4-4756-83FF-0FA2A5A8826C}" name="time" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{6152D57E-22A4-4756-83FF-0FA2A5A8826C}" name="time" dataDxfId="9">
       <calculatedColumnFormula>data!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{03763A0D-A48C-4D52-886F-3E4E1070B03F}" name="winter" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{03763A0D-A48C-4D52-886F-3E4E1070B03F}" name="winter" dataDxfId="8">
       <calculatedColumnFormula>AVERAGE(data!P4:R4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{71CCAC2C-5701-474F-9EC1-E2F89CC65AAC}" name="summer" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{71CCAC2C-5701-474F-9EC1-E2F89CC65AAC}" name="summer" dataDxfId="7">
       <calculatedColumnFormula>AVERAGE(data!S4:U4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -384,22 +356,22 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{65500618-7955-4477-BB55-B536E81F0228}" name="Tableau6" displayName="Tableau6" ref="A1:E97" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{65500618-7955-4477-BB55-B536E81F0228}" name="Tableau6" displayName="Tableau6" ref="A1:E97" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E97" xr:uid="{65500618-7955-4477-BB55-B536E81F0228}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0961E0D0-891A-498A-A97C-97FD88EDA497}" name="Courbe N1 winter" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{0961E0D0-891A-498A-A97C-97FD88EDA497}" name="Courbe N1 winter" dataDxfId="4">
       <calculatedColumnFormula>Tableau14[[#This Row],[winter]]*tests!$G$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E7E512C2-6011-4E3C-843A-EB7AFE4B64D0}" name="Courbe N1 winter avec valeur normalisée" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{E7E512C2-6011-4E3C-843A-EB7AFE4B64D0}" name="Courbe N1 winter avec valeur normalisée" dataDxfId="3">
       <calculatedColumnFormula>Tableau6[[#This Row],[Courbe N1 winter]]/(tests!$G$13/1000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{60EA1D1C-592A-452F-8891-9A2A53F3EFED}" name="Courbe 55 summer" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{60EA1D1C-592A-452F-8891-9A2A53F3EFED}" name="Courbe 55 summer" dataDxfId="2">
       <calculatedColumnFormula>Tableau1[[#This Row],[summer]]*$M$27</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6BF445AF-DBBF-42AC-8A36-DAEF4B510253}" name="Courbe 55 summer avec valeur normalisée" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{6BF445AF-DBBF-42AC-8A36-DAEF4B510253}" name="Courbe 55 summer avec valeur normalisée" dataDxfId="1">
       <calculatedColumnFormula>Tableau6[[#This Row],[Courbe 55 summer]]/($M$30/1000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{46E29576-C0F4-498B-BC37-5C2F6F037758}" name="Courbe N5" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{46E29576-C0F4-498B-BC37-5C2F6F037758}" name="Courbe N5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6365,7 +6337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9921FF-EDEB-4738-9EBD-B5B1C5CFF1DC}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -7738,7 +7710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB6BFC7-0142-480D-8D84-01C7C2FAB150}">
   <dimension ref="A1:AB99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>

</xml_diff>